<commit_message>
Update test for RT importer
</commit_message>
<xml_diff>
--- a/django_project/geosight/importer/tests/importers/_fixtures/excel_wide_related_table.xlsx
+++ b/django_project/geosight/importer/tests/importers/_fixtures/excel_wide_related_table.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="13">
   <si>
     <t xml:space="preserve">geom_code</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t xml:space="preserve">DateFormat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group</t>
   </si>
   <si>
     <t xml:space="preserve">A</t>
@@ -181,10 +184,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H24" activeCellId="0" sqref="H24"/>
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -193,6 +196,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.4"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -211,10 +215,13 @@
       <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
@@ -226,12 +233,15 @@
         <v>44562</v>
       </c>
       <c r="E2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>2</v>
@@ -243,12 +253,15 @@
         <v>44562</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>3</v>
@@ -260,12 +273,13 @@
         <v>44562</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>9</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>4</v>
@@ -277,12 +291,15 @@
         <v>44562</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>3</v>
@@ -294,12 +311,15 @@
         <v>44562</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>2</v>
@@ -311,12 +331,13 @@
         <v>44927</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>10</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" s="5" t="n">
         <v>1</v>
@@ -328,12 +349,15 @@
         <v>44927</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="5" t="n">
         <v>0</v>
@@ -345,12 +369,15 @@
         <v>44927</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="5" t="n">
         <v>1</v>
@@ -362,8 +389,9 @@
         <v>44927</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>6</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="F10" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="2"/>
@@ -422,7 +450,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
Handling null value of RT to be queried as blank (#324)
* Handling null value of RT to be queried as blank

* Update blank on single selection

* Update E2E project to handle blank RT data

* Update test for RT importer

* Fix tests

* Fix tests
</commit_message>
<xml_diff>
--- a/django_project/geosight/importer/tests/importers/_fixtures/excel_wide_related_table.xlsx
+++ b/django_project/geosight/importer/tests/importers/_fixtures/excel_wide_related_table.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="13">
   <si>
     <t xml:space="preserve">geom_code</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t xml:space="preserve">DateFormat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Group</t>
   </si>
   <si>
     <t xml:space="preserve">A</t>
@@ -181,10 +184,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E29"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H24" activeCellId="0" sqref="H24"/>
+      <selection pane="topLeft" activeCell="F10" activeCellId="0" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -193,6 +196,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.4"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -211,10 +215,13 @@
       <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="0" t="n">
         <v>1</v>
@@ -226,12 +233,15 @@
         <v>44562</v>
       </c>
       <c r="E2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>2</v>
@@ -243,12 +253,15 @@
         <v>44562</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>3</v>
@@ -260,12 +273,13 @@
         <v>44562</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>9</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>4</v>
@@ -277,12 +291,15 @@
         <v>44562</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>3</v>
@@ -294,12 +311,15 @@
         <v>44562</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>2</v>
@@ -311,12 +331,13 @@
         <v>44927</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>10</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="F7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B8" s="5" t="n">
         <v>1</v>
@@ -328,12 +349,15 @@
         <v>44927</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" s="5" t="n">
         <v>0</v>
@@ -345,12 +369,15 @@
         <v>44927</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" s="5" t="n">
         <v>1</v>
@@ -362,8 +389,9 @@
         <v>44927</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>6</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="F10" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D12" s="2"/>
@@ -422,7 +450,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>